<commit_message>
changing availability for islands
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RES_HeatSav_Trans.xlsx
+++ b/SubRES_TMPL/SubRes_RES_HeatSav_Trans.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olex\(^_^)\ResLab\Modelling\TIMES\TIMES-DK\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998D62CB-798F-449E-8FCE-9DAEC6C42BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="180" windowWidth="16605" windowHeight="6210" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4575" yWindow="2805" windowWidth="28800" windowHeight="15375" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="18" r:id="rId1"/>
@@ -28,12 +29,23 @@
     <definedName name="VARWSTBO">'[2]O&amp;M waste '!$D$5</definedName>
     <definedName name="VARWSTBP">'[2]O&amp;M waste '!$D$4</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="156">
   <si>
     <t>Individual</t>
   </si>
@@ -490,6 +502,18 @@
   <si>
     <t>Added AVA table for compatibility with STM</t>
   </si>
+  <si>
+    <t>DKISLBH</t>
+  </si>
+  <si>
+    <t>DKISL1</t>
+  </si>
+  <si>
+    <t>DKISL2</t>
+  </si>
+  <si>
+    <t>DKISL3</t>
+  </si>
 </sst>
 </file>
 
@@ -799,7 +823,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="64">
+  <fills count="66">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1141,6 +1165,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="44"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5076,7 +5112,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="172">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -5223,14 +5259,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1538" applyFont="1"/>
     <xf numFmtId="0" fontId="38" fillId="28" borderId="0" xfId="1538" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="31" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2578" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2578"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2578" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="63" borderId="22" xfId="2578" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5239,6 +5278,54 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="51" xfId="436" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="436" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" xfId="436" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="72" xfId="436" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
@@ -5253,34 +5340,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
@@ -5289,46 +5352,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="51" xfId="436" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="436" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" xfId="436" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="72" xfId="436" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2578" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2578"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2578" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="63" borderId="22" xfId="2578" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="2578" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="65" borderId="22" xfId="2578" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="65" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2580">
     <cellStyle name="20 % - Markeringsfarve1" xfId="1539" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -9214,17 +9252,17 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.59765625" style="108" customWidth="1"/>
-    <col min="2" max="2" width="15.73046875" style="108" customWidth="1"/>
-    <col min="3" max="3" width="13.86328125" style="108" customWidth="1"/>
-    <col min="4" max="4" width="19.86328125" style="108" customWidth="1"/>
-    <col min="5" max="5" width="60.265625" style="108" customWidth="1"/>
-    <col min="6" max="16384" width="9.1328125" style="108"/>
+    <col min="1" max="1" width="11.5703125" style="108" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="108" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="108" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="108" customWidth="1"/>
+    <col min="5" max="5" width="60.28515625" style="108" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="108"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="121" t="s">
         <v>121</v>
       </c>
@@ -9241,7 +9279,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="123" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" s="123" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="122">
         <v>42992</v>
       </c>
@@ -9259,7 +9297,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="123" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" s="123" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="122">
         <v>42814</v>
       </c>
@@ -9277,7 +9315,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="123" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" s="123" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="122">
         <v>42479</v>
       </c>
@@ -9288,7 +9326,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="123" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" s="123" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="122">
         <v>42479</v>
       </c>
@@ -9302,7 +9340,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="123" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" s="123" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="122">
         <v>42264</v>
       </c>
@@ -9336,20 +9374,20 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="127"/>
+    <col min="1" max="1" width="9.140625" style="127"/>
     <col min="2" max="2" width="24" style="127" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="138.3984375" style="127" customWidth="1"/>
-    <col min="4" max="16384" width="9.1328125" style="127"/>
+    <col min="3" max="3" width="138.42578125" style="127" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="127"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="126" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" s="128" t="s">
         <v>134</v>
       </c>
@@ -9357,15 +9395,15 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="128" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="128"/>
     </row>
-    <row r="6" spans="2:3" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="128" t="s">
         <v>136</v>
       </c>
@@ -9373,18 +9411,18 @@
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="128"/>
     </row>
-    <row r="8" spans="2:3" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="129" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="128"/>
     </row>
-    <row r="10" spans="2:3" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="130" t="s">
         <v>139</v>
       </c>
@@ -9392,7 +9430,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="132" t="s">
         <v>140</v>
       </c>
@@ -9416,52 +9454,77 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83D6AC78-F220-49AE-89C1-010838484A04}">
-  <dimension ref="B2:E4"/>
+  <dimension ref="B2:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B2" s="167" t="s">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="134" t="s">
         <v>147</v>
       </c>
-      <c r="C2" s="168"/>
-      <c r="D2" s="169"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="136"/>
       <c r="E2" s="108"/>
     </row>
-    <row r="3" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="170" t="s">
+    <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="137" t="s">
         <v>148</v>
       </c>
-      <c r="C3" s="170" t="s">
+      <c r="C3" s="137" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="170" t="s">
+      <c r="D3" s="137" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="171" t="s">
+      <c r="E3" s="172" t="s">
+        <v>152</v>
+      </c>
+      <c r="F3" s="173" t="s">
+        <v>153</v>
+      </c>
+      <c r="G3" s="173" t="s">
+        <v>154</v>
+      </c>
+      <c r="H3" s="173" t="s">
+        <v>155</v>
+      </c>
+      <c r="I3" s="171" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="108">
         <v>0</v>
       </c>
-      <c r="C4" s="168">
+      <c r="C4" s="135">
         <v>1</v>
       </c>
-      <c r="D4" s="168">
+      <c r="D4" s="135">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
         <v>149</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9476,24 +9539,24 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1328125" style="108" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="57.86328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="34.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="108" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="57.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.73046875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
@@ -9516,7 +9579,7 @@
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
     </row>
-    <row r="4" spans="2:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
@@ -9555,7 +9618,7 @@
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
     </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
       <c r="C5" s="6" t="s">
         <v>13</v>
@@ -9594,7 +9657,7 @@
       <c r="S5" s="6"/>
       <c r="T5" s="6"/>
     </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
         <v>13</v>
@@ -9633,7 +9696,7 @@
       <c r="S6" s="6"/>
       <c r="T6" s="6"/>
     </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
       <c r="C7" s="6" t="s">
         <v>13</v>
@@ -9672,7 +9735,7 @@
       <c r="S7" s="6"/>
       <c r="T7" s="6"/>
     </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
         <v>13</v>
@@ -9711,7 +9774,7 @@
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
     </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="C9" s="6" t="s">
         <v>13</v>
@@ -9750,7 +9813,7 @@
       <c r="S9" s="6"/>
       <c r="T9" s="6"/>
     </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="C10" s="6" t="s">
         <v>13</v>
@@ -9789,7 +9852,7 @@
       <c r="S10" s="6"/>
       <c r="T10" s="6"/>
     </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="C11" s="6" t="s">
         <v>13</v>
@@ -9828,7 +9891,7 @@
       <c r="S11" s="6"/>
       <c r="T11" s="6"/>
     </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
         <v>13</v>
@@ -9867,7 +9930,7 @@
       <c r="S12" s="6"/>
       <c r="T12" s="6"/>
     </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
       <c r="C13" s="6" t="s">
         <v>13</v>
@@ -9906,7 +9969,7 @@
       <c r="S13" s="6"/>
       <c r="T13" s="6"/>
     </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="C14" s="6" t="s">
         <v>13</v>
@@ -9945,7 +10008,7 @@
       <c r="S14" s="6"/>
       <c r="T14" s="6"/>
     </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="C15" s="6" t="s">
         <v>13</v>
@@ -9984,7 +10047,7 @@
       <c r="S15" s="6"/>
       <c r="T15" s="6"/>
     </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
         <v>13</v>
@@ -10023,7 +10086,7 @@
       <c r="S16" s="6"/>
       <c r="T16" s="6"/>
     </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" s="14"/>
       <c r="C17" s="14" t="s">
         <v>13</v>
@@ -10058,7 +10121,7 @@
       <c r="S17" s="6"/>
       <c r="T17" s="6"/>
     </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="5" t="s">
@@ -10095,7 +10158,7 @@
       <c r="S18" s="6"/>
       <c r="T18" s="6"/>
     </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="5" t="s">
@@ -10132,7 +10195,7 @@
       <c r="S19" s="6"/>
       <c r="T19" s="6"/>
     </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="5" t="s">
@@ -10169,7 +10232,7 @@
       <c r="S20" s="6"/>
       <c r="T20" s="6"/>
     </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="5" t="s">
@@ -10206,7 +10269,7 @@
       <c r="S21" s="6"/>
       <c r="T21" s="6"/>
     </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="5" t="s">
@@ -10243,7 +10306,7 @@
       <c r="S22" s="6"/>
       <c r="T22" s="6"/>
     </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="5" t="s">
@@ -10280,7 +10343,7 @@
       <c r="S23" s="6"/>
       <c r="T23" s="6"/>
     </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="5" t="s">
@@ -10317,7 +10380,7 @@
       <c r="S24" s="4"/>
       <c r="T24" s="4"/>
     </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="5" t="s">
@@ -10354,7 +10417,7 @@
       <c r="S25" s="4"/>
       <c r="T25" s="4"/>
     </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="5" t="s">
@@ -10391,7 +10454,7 @@
       <c r="S26" s="4"/>
       <c r="T26" s="4"/>
     </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="5" t="s">
@@ -10428,7 +10491,7 @@
       <c r="S27" s="4"/>
       <c r="T27" s="4"/>
     </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="5" t="s">
@@ -10465,7 +10528,7 @@
       <c r="S28" s="4"/>
       <c r="T28" s="4"/>
     </row>
-    <row r="29" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
       <c r="D29" s="16" t="s">
@@ -10502,7 +10565,7 @@
       <c r="S29" s="4"/>
       <c r="T29" s="4"/>
     </row>
-    <row r="30" spans="2:20" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="5" t="s">
@@ -10535,7 +10598,7 @@
       <c r="O30" s="6"/>
       <c r="P30" s="6"/>
     </row>
-    <row r="31" spans="2:20" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="5" t="s">
@@ -10568,7 +10631,7 @@
       <c r="O31" s="6"/>
       <c r="P31" s="6"/>
     </row>
-    <row r="32" spans="2:20" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="D32" s="5" t="s">
@@ -10601,7 +10664,7 @@
       <c r="O32" s="6"/>
       <c r="P32" s="6"/>
     </row>
-    <row r="33" spans="2:20" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="5" t="s">
@@ -10634,7 +10697,7 @@
       <c r="O33" s="6"/>
       <c r="P33" s="6"/>
     </row>
-    <row r="34" spans="2:20" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34" s="5" t="s">
@@ -10667,7 +10730,7 @@
       <c r="O34" s="6"/>
       <c r="P34" s="6"/>
     </row>
-    <row r="35" spans="2:20" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="5" t="s">
@@ -10700,7 +10763,7 @@
       <c r="O35" s="6"/>
       <c r="P35" s="6"/>
     </row>
-    <row r="36" spans="2:20" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
       <c r="D36" s="5" t="s">
@@ -10733,7 +10796,7 @@
       <c r="O36" s="6"/>
       <c r="P36" s="6"/>
     </row>
-    <row r="37" spans="2:20" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
       <c r="D37" s="5" t="s">
@@ -10766,7 +10829,7 @@
       <c r="O37" s="6"/>
       <c r="P37" s="6"/>
     </row>
-    <row r="38" spans="2:20" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
       <c r="D38" s="5" t="s">
@@ -10799,7 +10862,7 @@
       <c r="O38" s="6"/>
       <c r="P38" s="6"/>
     </row>
-    <row r="39" spans="2:20" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
       <c r="D39" s="5" t="s">
@@ -10832,7 +10895,7 @@
       <c r="O39" s="6"/>
       <c r="P39" s="6"/>
     </row>
-    <row r="40" spans="2:20" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
       <c r="D40" s="5" t="s">
@@ -10865,7 +10928,7 @@
       <c r="O40" s="6"/>
       <c r="P40" s="6"/>
     </row>
-    <row r="41" spans="2:20" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="14"/>
       <c r="C41" s="14"/>
       <c r="D41" s="16" t="s">
@@ -10898,7 +10961,7 @@
       <c r="O41" s="6"/>
       <c r="P41" s="6"/>
     </row>
-    <row r="42" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B42" s="6"/>
       <c r="C42" s="6" t="s">
         <v>13</v>
@@ -10937,7 +11000,7 @@
       <c r="S42" s="4"/>
       <c r="T42" s="4"/>
     </row>
-    <row r="43" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B43" s="4"/>
       <c r="C43" s="4" t="s">
         <v>13</v>
@@ -10976,7 +11039,7 @@
       <c r="S43" s="4"/>
       <c r="T43" s="4"/>
     </row>
-    <row r="44" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B44" s="4"/>
       <c r="C44" s="4" t="s">
         <v>13</v>
@@ -11015,7 +11078,7 @@
       <c r="S44" s="4"/>
       <c r="T44" s="4"/>
     </row>
-    <row r="45" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B45" s="4"/>
       <c r="C45" s="4" t="s">
         <v>13</v>
@@ -11049,7 +11112,7 @@
       <c r="N45" s="18"/>
       <c r="O45" s="6"/>
     </row>
-    <row r="46" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B46" s="4"/>
       <c r="C46" s="4" t="s">
         <v>13</v>
@@ -11083,7 +11146,7 @@
       <c r="N46" s="6"/>
       <c r="O46" s="6"/>
     </row>
-    <row r="47" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B47" s="4"/>
       <c r="C47" s="4" t="s">
         <v>13</v>
@@ -11117,7 +11180,7 @@
       <c r="N47" s="6"/>
       <c r="O47" s="6"/>
     </row>
-    <row r="48" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="48" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B48" s="4"/>
       <c r="C48" s="4" t="s">
         <v>13</v>
@@ -11151,7 +11214,7 @@
       <c r="N48" s="6"/>
       <c r="O48" s="6"/>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B49" s="4"/>
       <c r="C49" s="4" t="s">
         <v>13</v>
@@ -11185,7 +11248,7 @@
       <c r="N49" s="6"/>
       <c r="O49" s="6"/>
     </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B50" s="4"/>
       <c r="C50" s="4" t="s">
         <v>13</v>
@@ -11219,7 +11282,7 @@
       <c r="N50" s="6"/>
       <c r="O50" s="6"/>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B51" s="4"/>
       <c r="C51" s="4" t="s">
         <v>13</v>
@@ -11253,7 +11316,7 @@
       <c r="N51" s="6"/>
       <c r="O51" s="4"/>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B52" s="4"/>
       <c r="C52" s="4" t="s">
         <v>13</v>
@@ -11287,7 +11350,7 @@
       <c r="N52" s="6"/>
       <c r="O52" s="4"/>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B53" s="6"/>
       <c r="C53" s="6" t="s">
         <v>13</v>
@@ -11321,7 +11384,7 @@
       <c r="N53" s="6"/>
       <c r="O53" s="4"/>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B54" s="14"/>
       <c r="C54" s="14" t="s">
         <v>13</v>
@@ -11351,7 +11414,7 @@
       <c r="N54" s="6"/>
       <c r="O54" s="4"/>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="5" t="s">
@@ -11383,7 +11446,7 @@
       <c r="N55" s="6"/>
       <c r="O55" s="4"/>
     </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="5" t="s">
@@ -11415,7 +11478,7 @@
       <c r="N56" s="6"/>
       <c r="O56" s="4"/>
     </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="5" t="s">
@@ -11447,7 +11510,7 @@
       <c r="N57" s="6"/>
       <c r="O57" s="4"/>
     </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="5" t="s">
@@ -11479,7 +11542,7 @@
       <c r="N58" s="6"/>
       <c r="O58" s="4"/>
     </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="5" t="s">
@@ -11511,7 +11574,7 @@
       <c r="N59" s="6"/>
       <c r="O59" s="4"/>
     </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B60" s="4"/>
       <c r="C60" s="6"/>
       <c r="D60" s="5" t="s">
@@ -11543,7 +11606,7 @@
       <c r="N60" s="6"/>
       <c r="O60" s="4"/>
     </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="5" t="s">
@@ -11574,7 +11637,7 @@
       <c r="M61" s="5"/>
       <c r="N61" s="6"/>
     </row>
-    <row r="62" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="5" t="s">
@@ -11605,7 +11668,7 @@
       <c r="M62" s="5"/>
       <c r="N62" s="6"/>
     </row>
-    <row r="63" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="5" t="s">
@@ -11636,7 +11699,7 @@
       <c r="M63" s="5"/>
       <c r="N63" s="6"/>
     </row>
-    <row r="64" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="5" t="s">
@@ -11667,7 +11730,7 @@
       <c r="M64" s="5"/>
       <c r="N64" s="6"/>
     </row>
-    <row r="65" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="65" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="5" t="s">
@@ -11698,7 +11761,7 @@
       <c r="M65" s="5"/>
       <c r="N65" s="6"/>
     </row>
-    <row r="66" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="66" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B66" s="14"/>
       <c r="C66" s="14"/>
       <c r="D66" s="16" t="s">
@@ -11729,7 +11792,7 @@
       <c r="M66" s="5"/>
       <c r="N66" s="6"/>
     </row>
-    <row r="67" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
       <c r="D67" s="5" t="s">
@@ -11762,7 +11825,7 @@
       <c r="O67" s="13"/>
       <c r="P67" s="6"/>
     </row>
-    <row r="68" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
       <c r="D68" s="5" t="s">
@@ -11796,7 +11859,7 @@
       <c r="P68" s="6"/>
       <c r="Q68" s="108"/>
     </row>
-    <row r="69" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
       <c r="D69" s="5" t="s">
@@ -11830,7 +11893,7 @@
       <c r="P69" s="6"/>
       <c r="Q69" s="108"/>
     </row>
-    <row r="70" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
       <c r="D70" s="5" t="s">
@@ -11864,7 +11927,7 @@
       <c r="P70" s="6"/>
       <c r="Q70" s="108"/>
     </row>
-    <row r="71" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
       <c r="D71" s="5" t="s">
@@ -11898,7 +11961,7 @@
       <c r="P71" s="6"/>
       <c r="Q71" s="108"/>
     </row>
-    <row r="72" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
       <c r="D72" s="5" t="s">
@@ -11932,7 +11995,7 @@
       <c r="P72" s="6"/>
       <c r="Q72" s="108"/>
     </row>
-    <row r="73" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
       <c r="D73" s="5" t="s">
@@ -11966,7 +12029,7 @@
       <c r="P73" s="6"/>
       <c r="Q73" s="108"/>
     </row>
-    <row r="74" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
       <c r="D74" s="5" t="s">
@@ -12000,7 +12063,7 @@
       <c r="P74" s="6"/>
       <c r="Q74" s="108"/>
     </row>
-    <row r="75" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
       <c r="D75" s="5" t="s">
@@ -12034,7 +12097,7 @@
       <c r="P75" s="6"/>
       <c r="Q75" s="108"/>
     </row>
-    <row r="76" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
       <c r="D76" s="5" t="s">
@@ -12068,7 +12131,7 @@
       <c r="P76" s="6"/>
       <c r="Q76" s="108"/>
     </row>
-    <row r="77" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
       <c r="D77" s="5" t="s">
@@ -12102,7 +12165,7 @@
       <c r="P77" s="6"/>
       <c r="Q77" s="108"/>
     </row>
-    <row r="78" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B78" s="14"/>
       <c r="C78" s="14"/>
       <c r="D78" s="16" t="s">
@@ -12136,7 +12199,7 @@
       <c r="P78" s="6"/>
       <c r="Q78" s="108"/>
     </row>
-    <row r="79" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="79" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B79" s="6"/>
       <c r="C79" s="6" t="s">
         <v>13</v>
@@ -12169,7 +12232,7 @@
       <c r="M79" s="5"/>
       <c r="N79" s="6"/>
     </row>
-    <row r="80" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="80" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B80" s="6"/>
       <c r="C80" s="6" t="s">
         <v>13</v>
@@ -12202,7 +12265,7 @@
       <c r="M80" s="5"/>
       <c r="N80" s="6"/>
     </row>
-    <row r="81" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="81" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B81" s="6"/>
       <c r="C81" s="6" t="s">
         <v>13</v>
@@ -12235,7 +12298,7 @@
       <c r="M81" s="5"/>
       <c r="N81" s="6"/>
     </row>
-    <row r="82" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="82" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B82" s="6"/>
       <c r="C82" s="6" t="s">
         <v>13</v>
@@ -12268,7 +12331,7 @@
       <c r="M82" s="5"/>
       <c r="N82" s="6"/>
     </row>
-    <row r="83" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="83" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B83" s="6"/>
       <c r="C83" s="6" t="s">
         <v>13</v>
@@ -12301,7 +12364,7 @@
       <c r="M83" s="5"/>
       <c r="N83" s="6"/>
     </row>
-    <row r="84" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="84" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B84" s="6"/>
       <c r="C84" s="6" t="s">
         <v>13</v>
@@ -12334,7 +12397,7 @@
       <c r="M84" s="5"/>
       <c r="N84" s="6"/>
     </row>
-    <row r="85" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="85" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B85" s="6"/>
       <c r="C85" s="6" t="s">
         <v>13</v>
@@ -12367,7 +12430,7 @@
       <c r="M85" s="5"/>
       <c r="N85" s="6"/>
     </row>
-    <row r="86" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="86" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B86" s="6"/>
       <c r="C86" s="6" t="s">
         <v>13</v>
@@ -12400,7 +12463,7 @@
       <c r="M86" s="5"/>
       <c r="N86" s="6"/>
     </row>
-    <row r="87" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="87" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B87" s="6"/>
       <c r="C87" s="6" t="s">
         <v>13</v>
@@ -12433,7 +12496,7 @@
       <c r="M87" s="5"/>
       <c r="N87" s="6"/>
     </row>
-    <row r="88" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="88" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B88" s="6"/>
       <c r="C88" s="6" t="s">
         <v>13</v>
@@ -12466,7 +12529,7 @@
       <c r="M88" s="5"/>
       <c r="N88" s="6"/>
     </row>
-    <row r="89" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="89" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B89" s="6"/>
       <c r="C89" s="6" t="s">
         <v>13</v>
@@ -12499,7 +12562,7 @@
       <c r="M89" s="5"/>
       <c r="N89" s="6"/>
     </row>
-    <row r="90" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="90" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B90" s="6"/>
       <c r="C90" s="6" t="s">
         <v>13</v>
@@ -12532,7 +12595,7 @@
       <c r="M90" s="5"/>
       <c r="N90" s="6"/>
     </row>
-    <row r="91" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="91" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B91" s="14"/>
       <c r="C91" s="14" t="s">
         <v>13</v>
@@ -12561,7 +12624,7 @@
       <c r="M91" s="5"/>
       <c r="N91" s="6"/>
     </row>
-    <row r="92" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="92" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="5" t="s">
@@ -12592,7 +12655,7 @@
       <c r="M92" s="5"/>
       <c r="N92" s="6"/>
     </row>
-    <row r="93" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="93" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
       <c r="D93" s="5" t="s">
@@ -12623,7 +12686,7 @@
       <c r="M93" s="5"/>
       <c r="N93" s="6"/>
     </row>
-    <row r="94" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="94" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
       <c r="D94" s="5" t="s">
@@ -12654,7 +12717,7 @@
       <c r="M94" s="5"/>
       <c r="N94" s="6"/>
     </row>
-    <row r="95" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="95" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
       <c r="D95" s="5" t="s">
@@ -12685,7 +12748,7 @@
       <c r="M95" s="5"/>
       <c r="N95" s="6"/>
     </row>
-    <row r="96" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="96" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="5" t="s">
@@ -12716,7 +12779,7 @@
       <c r="M96" s="5"/>
       <c r="N96" s="6"/>
     </row>
-    <row r="97" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="97" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B97" s="4"/>
       <c r="C97" s="6"/>
       <c r="D97" s="5" t="s">
@@ -12747,7 +12810,7 @@
       <c r="M97" s="5"/>
       <c r="N97" s="6"/>
     </row>
-    <row r="98" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="98" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
       <c r="D98" s="5" t="s">
@@ -12778,7 +12841,7 @@
       <c r="M98" s="5"/>
       <c r="N98" s="6"/>
     </row>
-    <row r="99" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="99" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
       <c r="D99" s="5" t="s">
@@ -12809,7 +12872,7 @@
       <c r="M99" s="5"/>
       <c r="N99" s="6"/>
     </row>
-    <row r="100" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="100" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
       <c r="D100" s="5" t="s">
@@ -12840,7 +12903,7 @@
       <c r="M100" s="5"/>
       <c r="N100" s="6"/>
     </row>
-    <row r="101" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="101" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
       <c r="D101" s="5" t="s">
@@ -12871,7 +12934,7 @@
       <c r="M101" s="5"/>
       <c r="N101" s="6"/>
     </row>
-    <row r="102" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="102" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
       <c r="D102" s="5" t="s">
@@ -12902,7 +12965,7 @@
       <c r="M102" s="5"/>
       <c r="N102" s="6"/>
     </row>
-    <row r="103" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="103" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B103" s="14"/>
       <c r="C103" s="14"/>
       <c r="D103" s="16" t="s">
@@ -12933,7 +12996,7 @@
       <c r="M103" s="5"/>
       <c r="N103" s="6"/>
     </row>
-    <row r="104" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="104" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B104" s="6"/>
       <c r="C104" s="6"/>
       <c r="D104" s="5" t="s">
@@ -12964,7 +13027,7 @@
       <c r="M104" s="5"/>
       <c r="N104" s="6"/>
     </row>
-    <row r="105" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="105" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D105" s="5" t="s">
         <v>52</v>
       </c>
@@ -12993,7 +13056,7 @@
       <c r="M105" s="5"/>
       <c r="N105" s="6"/>
     </row>
-    <row r="106" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="106" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D106" s="5" t="s">
         <v>52</v>
       </c>
@@ -13022,7 +13085,7 @@
       <c r="M106" s="5"/>
       <c r="N106" s="6"/>
     </row>
-    <row r="107" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="107" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D107" s="5" t="s">
         <v>52</v>
       </c>
@@ -13051,7 +13114,7 @@
       <c r="M107" s="5"/>
       <c r="N107" s="6"/>
     </row>
-    <row r="108" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="108" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D108" s="5" t="s">
         <v>52</v>
       </c>
@@ -13080,7 +13143,7 @@
       <c r="M108" s="5"/>
       <c r="N108" s="6"/>
     </row>
-    <row r="109" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="109" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D109" s="5" t="s">
         <v>52</v>
       </c>
@@ -13109,7 +13172,7 @@
       <c r="M109" s="5"/>
       <c r="N109" s="6"/>
     </row>
-    <row r="110" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="110" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D110" s="5" t="s">
         <v>52</v>
       </c>
@@ -13138,7 +13201,7 @@
       <c r="M110" s="5"/>
       <c r="N110" s="6"/>
     </row>
-    <row r="111" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="111" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D111" s="5" t="s">
         <v>52</v>
       </c>
@@ -13167,7 +13230,7 @@
       <c r="M111" s="5"/>
       <c r="N111" s="6"/>
     </row>
-    <row r="112" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="112" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D112" s="5" t="s">
         <v>52</v>
       </c>
@@ -13196,7 +13259,7 @@
       <c r="M112" s="5"/>
       <c r="N112" s="6"/>
     </row>
-    <row r="113" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="113" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D113" s="5" t="s">
         <v>52</v>
       </c>
@@ -13225,7 +13288,7 @@
       <c r="M113" s="5"/>
       <c r="N113" s="6"/>
     </row>
-    <row r="114" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="114" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D114" s="5" t="s">
         <v>52</v>
       </c>
@@ -13254,7 +13317,7 @@
       <c r="M114" s="5"/>
       <c r="N114" s="6"/>
     </row>
-    <row r="115" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="115" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B115" s="14"/>
       <c r="C115" s="14"/>
       <c r="D115" s="16" t="s">
@@ -13285,7 +13348,7 @@
       <c r="M115" s="5"/>
       <c r="N115" s="6"/>
     </row>
-    <row r="116" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="116" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B116" s="6"/>
       <c r="C116" s="6"/>
       <c r="D116" s="6"/>
@@ -13299,35 +13362,35 @@
       <c r="M116" s="6"/>
       <c r="N116" s="6"/>
     </row>
-    <row r="117" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="117" spans="2:14" x14ac:dyDescent="0.25">
       <c r="J117" s="6"/>
       <c r="K117" s="6"/>
       <c r="L117" s="6"/>
       <c r="M117" s="6"/>
       <c r="N117" s="6"/>
     </row>
-    <row r="118" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="118" spans="2:14" x14ac:dyDescent="0.25">
       <c r="J118" s="6"/>
       <c r="K118" s="6"/>
       <c r="L118" s="6"/>
       <c r="M118" s="6"/>
       <c r="N118" s="6"/>
     </row>
-    <row r="119" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="119" spans="2:14" x14ac:dyDescent="0.25">
       <c r="J119" s="6"/>
       <c r="K119" s="6"/>
       <c r="L119" s="6"/>
       <c r="M119" s="6"/>
       <c r="N119" s="6"/>
     </row>
-    <row r="120" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="120" spans="2:14" x14ac:dyDescent="0.25">
       <c r="J120" s="6"/>
       <c r="K120" s="6"/>
       <c r="L120" s="6"/>
       <c r="M120" s="6"/>
       <c r="N120" s="6"/>
     </row>
-    <row r="121" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="121" spans="2:14" x14ac:dyDescent="0.25">
       <c r="J121" s="6"/>
       <c r="K121" s="6"/>
       <c r="L121" s="6"/>
@@ -13352,25 +13415,25 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="4"/>
-    <col min="2" max="2" width="25.59765625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.3984375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="25.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="4" customWidth="1"/>
     <col min="4" max="5" width="13" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="24" width="9.1328125" style="4"/>
-    <col min="25" max="25" width="7.265625" style="4" customWidth="1"/>
-    <col min="26" max="29" width="9.1328125" style="4"/>
-    <col min="30" max="30" width="12.265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.3984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.73046875" style="4" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.3984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.73046875" style="4" bestFit="1" customWidth="1"/>
-    <col min="36" max="16384" width="9.1328125" style="4"/>
+    <col min="6" max="24" width="9.140625" style="4"/>
+    <col min="25" max="25" width="7.28515625" style="4" customWidth="1"/>
+    <col min="26" max="29" width="9.140625" style="4"/>
+    <col min="30" max="30" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="36" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="108"/>
       <c r="B1" s="108"/>
       <c r="C1" s="108" t="s">
@@ -13401,7 +13464,7 @@
       <c r="Z1" s="108"/>
       <c r="AA1" s="108"/>
     </row>
-    <row r="2" spans="1:35" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="108"/>
       <c r="B2" s="108"/>
       <c r="C2" s="108"/>
@@ -13430,127 +13493,127 @@
       <c r="Z2" s="108"/>
       <c r="AA2" s="108"/>
     </row>
-    <row r="3" spans="1:35" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:35" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="108"/>
       <c r="B3" s="108"/>
-      <c r="C3" s="134" t="s">
+      <c r="C3" s="156" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="135"/>
-      <c r="E3" s="135"/>
-      <c r="F3" s="135"/>
-      <c r="G3" s="135"/>
-      <c r="H3" s="135"/>
-      <c r="I3" s="135"/>
-      <c r="J3" s="135"/>
-      <c r="K3" s="135"/>
-      <c r="L3" s="135"/>
-      <c r="M3" s="135"/>
-      <c r="N3" s="135"/>
-      <c r="O3" s="135"/>
-      <c r="P3" s="135"/>
-      <c r="Q3" s="135"/>
-      <c r="R3" s="135"/>
-      <c r="S3" s="135"/>
-      <c r="T3" s="135"/>
-      <c r="U3" s="135"/>
-      <c r="V3" s="135"/>
-      <c r="W3" s="135"/>
-      <c r="X3" s="135"/>
-      <c r="Y3" s="135"/>
-      <c r="Z3" s="136"/>
+      <c r="D3" s="157"/>
+      <c r="E3" s="157"/>
+      <c r="F3" s="157"/>
+      <c r="G3" s="157"/>
+      <c r="H3" s="157"/>
+      <c r="I3" s="157"/>
+      <c r="J3" s="157"/>
+      <c r="K3" s="157"/>
+      <c r="L3" s="157"/>
+      <c r="M3" s="157"/>
+      <c r="N3" s="157"/>
+      <c r="O3" s="157"/>
+      <c r="P3" s="157"/>
+      <c r="Q3" s="157"/>
+      <c r="R3" s="157"/>
+      <c r="S3" s="157"/>
+      <c r="T3" s="157"/>
+      <c r="U3" s="157"/>
+      <c r="V3" s="157"/>
+      <c r="W3" s="157"/>
+      <c r="X3" s="157"/>
+      <c r="Y3" s="157"/>
+      <c r="Z3" s="158"/>
       <c r="AA3" s="108"/>
-      <c r="AD3" s="137" t="s">
+      <c r="AD3" s="140" t="s">
         <v>59</v>
       </c>
-      <c r="AE3" s="138"/>
-      <c r="AF3" s="138"/>
-      <c r="AG3" s="138"/>
-      <c r="AH3" s="138"/>
-      <c r="AI3" s="139"/>
-    </row>
-    <row r="4" spans="1:35" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="AE3" s="141"/>
+      <c r="AF3" s="141"/>
+      <c r="AG3" s="141"/>
+      <c r="AH3" s="141"/>
+      <c r="AI3" s="142"/>
+    </row>
+    <row r="4" spans="1:35" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="108"/>
       <c r="B4" s="108"/>
-      <c r="C4" s="140" t="s">
+      <c r="C4" s="159" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="141"/>
-      <c r="E4" s="141"/>
-      <c r="F4" s="141"/>
-      <c r="G4" s="141"/>
-      <c r="H4" s="141"/>
-      <c r="I4" s="141"/>
-      <c r="J4" s="141"/>
-      <c r="K4" s="141"/>
-      <c r="L4" s="141"/>
-      <c r="M4" s="141"/>
-      <c r="N4" s="141"/>
-      <c r="O4" s="142" t="s">
+      <c r="D4" s="160"/>
+      <c r="E4" s="160"/>
+      <c r="F4" s="160"/>
+      <c r="G4" s="160"/>
+      <c r="H4" s="160"/>
+      <c r="I4" s="160"/>
+      <c r="J4" s="160"/>
+      <c r="K4" s="160"/>
+      <c r="L4" s="160"/>
+      <c r="M4" s="160"/>
+      <c r="N4" s="160"/>
+      <c r="O4" s="161" t="s">
         <v>11</v>
       </c>
-      <c r="P4" s="141"/>
-      <c r="Q4" s="141"/>
-      <c r="R4" s="141"/>
-      <c r="S4" s="141"/>
-      <c r="T4" s="141"/>
-      <c r="U4" s="141"/>
-      <c r="V4" s="141"/>
-      <c r="W4" s="141"/>
-      <c r="X4" s="141"/>
-      <c r="Y4" s="141"/>
-      <c r="Z4" s="143"/>
+      <c r="P4" s="160"/>
+      <c r="Q4" s="160"/>
+      <c r="R4" s="160"/>
+      <c r="S4" s="160"/>
+      <c r="T4" s="160"/>
+      <c r="U4" s="160"/>
+      <c r="V4" s="160"/>
+      <c r="W4" s="160"/>
+      <c r="X4" s="160"/>
+      <c r="Y4" s="160"/>
+      <c r="Z4" s="162"/>
       <c r="AA4" s="108"/>
       <c r="AD4" s="19"/>
       <c r="AE4" s="20"/>
-      <c r="AF4" s="144" t="s">
+      <c r="AF4" s="143" t="s">
         <v>56</v>
       </c>
-      <c r="AG4" s="145"/>
+      <c r="AG4" s="144"/>
       <c r="AH4" s="21" t="s">
         <v>57</v>
       </c>
       <c r="AI4" s="22"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="108"/>
       <c r="B5" s="108"/>
-      <c r="C5" s="153" t="s">
+      <c r="C5" s="163" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="146"/>
-      <c r="E5" s="146"/>
-      <c r="F5" s="146"/>
-      <c r="G5" s="154" t="s">
+      <c r="D5" s="164"/>
+      <c r="E5" s="164"/>
+      <c r="F5" s="164"/>
+      <c r="G5" s="165" t="s">
         <v>61</v>
       </c>
-      <c r="H5" s="146"/>
-      <c r="I5" s="146"/>
-      <c r="J5" s="155"/>
-      <c r="K5" s="146" t="s">
+      <c r="H5" s="164"/>
+      <c r="I5" s="164"/>
+      <c r="J5" s="166"/>
+      <c r="K5" s="164" t="s">
         <v>62</v>
       </c>
-      <c r="L5" s="146"/>
-      <c r="M5" s="146"/>
-      <c r="N5" s="146"/>
-      <c r="O5" s="156" t="s">
+      <c r="L5" s="164"/>
+      <c r="M5" s="164"/>
+      <c r="N5" s="164"/>
+      <c r="O5" s="169" t="s">
         <v>60</v>
       </c>
-      <c r="P5" s="146"/>
-      <c r="Q5" s="146"/>
-      <c r="R5" s="146"/>
-      <c r="S5" s="154" t="s">
+      <c r="P5" s="164"/>
+      <c r="Q5" s="164"/>
+      <c r="R5" s="164"/>
+      <c r="S5" s="165" t="s">
         <v>61</v>
       </c>
-      <c r="T5" s="146"/>
-      <c r="U5" s="146"/>
-      <c r="V5" s="155"/>
-      <c r="W5" s="146" t="s">
+      <c r="T5" s="164"/>
+      <c r="U5" s="164"/>
+      <c r="V5" s="166"/>
+      <c r="W5" s="164" t="s">
         <v>62</v>
       </c>
-      <c r="X5" s="146"/>
-      <c r="Y5" s="146"/>
-      <c r="Z5" s="147"/>
+      <c r="X5" s="164"/>
+      <c r="Y5" s="164"/>
+      <c r="Z5" s="170"/>
       <c r="AA5" s="108"/>
       <c r="AD5" s="23"/>
       <c r="AE5" s="6"/>
@@ -13567,59 +13630,59 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="108"/>
       <c r="B6" s="108"/>
-      <c r="C6" s="148" t="s">
+      <c r="C6" s="167" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="149"/>
-      <c r="E6" s="149" t="s">
+      <c r="D6" s="153"/>
+      <c r="E6" s="153" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="149"/>
-      <c r="G6" s="150" t="s">
+      <c r="F6" s="153"/>
+      <c r="G6" s="154" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="149"/>
-      <c r="I6" s="149" t="s">
+      <c r="H6" s="153"/>
+      <c r="I6" s="153" t="s">
         <v>66</v>
       </c>
-      <c r="J6" s="151"/>
-      <c r="K6" s="149" t="s">
+      <c r="J6" s="155"/>
+      <c r="K6" s="153" t="s">
         <v>65</v>
       </c>
-      <c r="L6" s="149"/>
-      <c r="M6" s="149" t="s">
+      <c r="L6" s="153"/>
+      <c r="M6" s="153" t="s">
         <v>66</v>
       </c>
-      <c r="N6" s="149"/>
+      <c r="N6" s="153"/>
       <c r="O6" s="152" t="s">
         <v>65</v>
       </c>
-      <c r="P6" s="149"/>
-      <c r="Q6" s="149" t="s">
+      <c r="P6" s="153"/>
+      <c r="Q6" s="153" t="s">
         <v>66</v>
       </c>
-      <c r="R6" s="149"/>
-      <c r="S6" s="150" t="s">
+      <c r="R6" s="153"/>
+      <c r="S6" s="154" t="s">
         <v>65</v>
       </c>
-      <c r="T6" s="149"/>
-      <c r="U6" s="149" t="s">
+      <c r="T6" s="153"/>
+      <c r="U6" s="153" t="s">
         <v>66</v>
       </c>
-      <c r="V6" s="151"/>
-      <c r="W6" s="149" t="s">
+      <c r="V6" s="155"/>
+      <c r="W6" s="153" t="s">
         <v>65</v>
       </c>
-      <c r="X6" s="149"/>
-      <c r="Y6" s="149" t="s">
+      <c r="X6" s="153"/>
+      <c r="Y6" s="153" t="s">
         <v>66</v>
       </c>
-      <c r="Z6" s="157"/>
+      <c r="Z6" s="168"/>
       <c r="AA6" s="108"/>
-      <c r="AD6" s="158" t="s">
+      <c r="AD6" s="147" t="s">
         <v>2</v>
       </c>
       <c r="AE6" s="25" t="s">
@@ -13638,7 +13701,7 @@
         <v>21.315135762203379</v>
       </c>
     </row>
-    <row r="7" spans="1:35" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="108"/>
       <c r="B7" s="108"/>
       <c r="C7" s="28" t="s">
@@ -13714,7 +13777,7 @@
         <v>68</v>
       </c>
       <c r="AA7" s="108"/>
-      <c r="AD7" s="159"/>
+      <c r="AD7" s="148"/>
       <c r="AE7" s="25" t="s">
         <v>4</v>
       </c>
@@ -13731,8 +13794,8 @@
         <v>15.84696230373755</v>
       </c>
     </row>
-    <row r="8" spans="1:35" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="161" t="s">
+    <row r="8" spans="1:35" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="138" t="s">
         <v>69</v>
       </c>
       <c r="B8" s="31" t="s">
@@ -13811,7 +13874,7 @@
         <v>1.8000000000000002E-2</v>
       </c>
       <c r="AA8" s="108"/>
-      <c r="AD8" s="160"/>
+      <c r="AD8" s="149"/>
       <c r="AE8" s="25" t="s">
         <v>0</v>
       </c>
@@ -13828,8 +13891,8 @@
         <v>11.550181131908179</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A9" s="162"/>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A9" s="139"/>
       <c r="B9" s="124" t="s">
         <v>77</v>
       </c>
@@ -13906,7 +13969,7 @@
         <v>1498.8565458526366</v>
       </c>
       <c r="AA9" s="108"/>
-      <c r="AD9" s="158" t="s">
+      <c r="AD9" s="147" t="s">
         <v>1</v>
       </c>
       <c r="AE9" s="25" t="s">
@@ -13925,8 +13988,8 @@
         <v>3.2947212563397263</v>
       </c>
     </row>
-    <row r="10" spans="1:35" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="162"/>
+    <row r="10" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="139"/>
       <c r="B10" s="41" t="s">
         <v>71</v>
       </c>
@@ -14003,7 +14066,7 @@
         <v>25.784078898824173</v>
       </c>
       <c r="AA10" s="108"/>
-      <c r="AD10" s="159"/>
+      <c r="AD10" s="148"/>
       <c r="AE10" s="25" t="s">
         <v>4</v>
       </c>
@@ -14020,8 +14083,8 @@
         <v>5.1367738966410732</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="164" t="s">
+    <row r="11" spans="1:35" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="145" t="s">
         <v>72</v>
       </c>
       <c r="B11" s="49" t="s">
@@ -14100,7 +14163,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="AA11" s="108"/>
-      <c r="AD11" s="163"/>
+      <c r="AD11" s="151"/>
       <c r="AE11" s="57" t="s">
         <v>0</v>
       </c>
@@ -14117,8 +14180,8 @@
         <v>0.35546674720410998</v>
       </c>
     </row>
-    <row r="12" spans="1:35" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="162"/>
+    <row r="12" spans="1:35" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="139"/>
       <c r="B12" s="124" t="s">
         <v>77</v>
       </c>
@@ -14196,8 +14259,8 @@
       </c>
       <c r="AA12" s="108"/>
     </row>
-    <row r="13" spans="1:35" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="165"/>
+    <row r="13" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="146"/>
       <c r="B13" s="41" t="s">
         <v>71</v>
       </c>
@@ -14275,8 +14338,8 @@
       </c>
       <c r="AA13" s="108"/>
     </row>
-    <row r="14" spans="1:35" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="162" t="s">
+    <row r="14" spans="1:35" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="139" t="s">
         <v>73</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -14355,17 +14418,17 @@
         <v>2.4694546524051571E-2</v>
       </c>
       <c r="AA14" s="108"/>
-      <c r="AD14" s="137" t="s">
+      <c r="AD14" s="140" t="s">
         <v>74</v>
       </c>
-      <c r="AE14" s="138"/>
-      <c r="AF14" s="138"/>
-      <c r="AG14" s="138"/>
-      <c r="AH14" s="138"/>
-      <c r="AI14" s="139"/>
-    </row>
-    <row r="15" spans="1:35" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="162"/>
+      <c r="AE14" s="141"/>
+      <c r="AF14" s="141"/>
+      <c r="AG14" s="141"/>
+      <c r="AH14" s="141"/>
+      <c r="AI14" s="142"/>
+    </row>
+    <row r="15" spans="1:35" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="139"/>
       <c r="B15" s="124" t="s">
         <v>77</v>
       </c>
@@ -14444,17 +14507,17 @@
       <c r="AA15" s="108"/>
       <c r="AD15" s="19"/>
       <c r="AE15" s="20"/>
-      <c r="AF15" s="144" t="s">
+      <c r="AF15" s="143" t="s">
         <v>56</v>
       </c>
-      <c r="AG15" s="145"/>
+      <c r="AG15" s="144"/>
       <c r="AH15" s="21" t="s">
         <v>57</v>
       </c>
       <c r="AI15" s="22"/>
     </row>
-    <row r="16" spans="1:35" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="166"/>
+    <row r="16" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="150"/>
       <c r="B16" s="41" t="s">
         <v>71</v>
       </c>
@@ -14546,7 +14609,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:35" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:35" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="75"/>
       <c r="B17" s="76"/>
       <c r="C17" s="76"/>
@@ -14574,7 +14637,7 @@
       <c r="Y17" s="76"/>
       <c r="Z17" s="76"/>
       <c r="AA17" s="6"/>
-      <c r="AD17" s="158" t="s">
+      <c r="AD17" s="147" t="s">
         <v>2</v>
       </c>
       <c r="AE17" s="25" t="s">
@@ -14593,7 +14656,7 @@
         <v>8.1202636786615034</v>
       </c>
     </row>
-    <row r="18" spans="1:35" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="75"/>
       <c r="B18" s="76"/>
       <c r="C18" s="76"/>
@@ -14621,7 +14684,7 @@
       <c r="Y18" s="76"/>
       <c r="Z18" s="76"/>
       <c r="AA18" s="6"/>
-      <c r="AD18" s="159"/>
+      <c r="AD18" s="148"/>
       <c r="AE18" s="25" t="s">
         <v>4</v>
       </c>
@@ -14638,37 +14701,37 @@
         <v>5.9452210330257413</v>
       </c>
     </row>
-    <row r="19" spans="1:35" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:35" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="108"/>
       <c r="B19" s="108"/>
-      <c r="C19" s="134" t="s">
+      <c r="C19" s="156" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="135"/>
-      <c r="E19" s="135"/>
-      <c r="F19" s="135"/>
-      <c r="G19" s="135"/>
-      <c r="H19" s="135"/>
-      <c r="I19" s="135"/>
-      <c r="J19" s="135"/>
-      <c r="K19" s="135"/>
-      <c r="L19" s="135"/>
-      <c r="M19" s="135"/>
-      <c r="N19" s="135"/>
-      <c r="O19" s="135"/>
-      <c r="P19" s="135"/>
-      <c r="Q19" s="135"/>
-      <c r="R19" s="135"/>
-      <c r="S19" s="135"/>
-      <c r="T19" s="135"/>
-      <c r="U19" s="135"/>
-      <c r="V19" s="135"/>
-      <c r="W19" s="135"/>
-      <c r="X19" s="135"/>
-      <c r="Y19" s="135"/>
-      <c r="Z19" s="136"/>
+      <c r="D19" s="157"/>
+      <c r="E19" s="157"/>
+      <c r="F19" s="157"/>
+      <c r="G19" s="157"/>
+      <c r="H19" s="157"/>
+      <c r="I19" s="157"/>
+      <c r="J19" s="157"/>
+      <c r="K19" s="157"/>
+      <c r="L19" s="157"/>
+      <c r="M19" s="157"/>
+      <c r="N19" s="157"/>
+      <c r="O19" s="157"/>
+      <c r="P19" s="157"/>
+      <c r="Q19" s="157"/>
+      <c r="R19" s="157"/>
+      <c r="S19" s="157"/>
+      <c r="T19" s="157"/>
+      <c r="U19" s="157"/>
+      <c r="V19" s="157"/>
+      <c r="W19" s="157"/>
+      <c r="X19" s="157"/>
+      <c r="Y19" s="157"/>
+      <c r="Z19" s="158"/>
       <c r="AA19" s="6"/>
-      <c r="AD19" s="160"/>
+      <c r="AD19" s="149"/>
       <c r="AE19" s="25" t="s">
         <v>0</v>
       </c>
@@ -14685,39 +14748,39 @@
         <v>4.4847162382110861</v>
       </c>
     </row>
-    <row r="20" spans="1:35" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:35" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="108"/>
       <c r="B20" s="108"/>
-      <c r="C20" s="140" t="s">
+      <c r="C20" s="159" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="141"/>
-      <c r="E20" s="141"/>
-      <c r="F20" s="141"/>
-      <c r="G20" s="141"/>
-      <c r="H20" s="141"/>
-      <c r="I20" s="141"/>
-      <c r="J20" s="141"/>
-      <c r="K20" s="141"/>
-      <c r="L20" s="141"/>
-      <c r="M20" s="141"/>
-      <c r="N20" s="141"/>
-      <c r="O20" s="142" t="s">
+      <c r="D20" s="160"/>
+      <c r="E20" s="160"/>
+      <c r="F20" s="160"/>
+      <c r="G20" s="160"/>
+      <c r="H20" s="160"/>
+      <c r="I20" s="160"/>
+      <c r="J20" s="160"/>
+      <c r="K20" s="160"/>
+      <c r="L20" s="160"/>
+      <c r="M20" s="160"/>
+      <c r="N20" s="160"/>
+      <c r="O20" s="161" t="s">
         <v>11</v>
       </c>
-      <c r="P20" s="141"/>
-      <c r="Q20" s="141"/>
-      <c r="R20" s="141"/>
-      <c r="S20" s="141"/>
-      <c r="T20" s="141"/>
-      <c r="U20" s="141"/>
-      <c r="V20" s="141"/>
-      <c r="W20" s="141"/>
-      <c r="X20" s="141"/>
-      <c r="Y20" s="141"/>
-      <c r="Z20" s="143"/>
+      <c r="P20" s="160"/>
+      <c r="Q20" s="160"/>
+      <c r="R20" s="160"/>
+      <c r="S20" s="160"/>
+      <c r="T20" s="160"/>
+      <c r="U20" s="160"/>
+      <c r="V20" s="160"/>
+      <c r="W20" s="160"/>
+      <c r="X20" s="160"/>
+      <c r="Y20" s="160"/>
+      <c r="Z20" s="162"/>
       <c r="AA20" s="108"/>
-      <c r="AD20" s="158" t="s">
+      <c r="AD20" s="147" t="s">
         <v>1</v>
       </c>
       <c r="AE20" s="25" t="s">
@@ -14736,47 +14799,47 @@
         <v>1.148592335548104</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" s="108"/>
       <c r="B21" s="108"/>
-      <c r="C21" s="153" t="s">
+      <c r="C21" s="163" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="146"/>
-      <c r="E21" s="146"/>
-      <c r="F21" s="146"/>
-      <c r="G21" s="154" t="s">
+      <c r="D21" s="164"/>
+      <c r="E21" s="164"/>
+      <c r="F21" s="164"/>
+      <c r="G21" s="165" t="s">
         <v>61</v>
       </c>
-      <c r="H21" s="146"/>
-      <c r="I21" s="146"/>
-      <c r="J21" s="155"/>
-      <c r="K21" s="146" t="s">
+      <c r="H21" s="164"/>
+      <c r="I21" s="164"/>
+      <c r="J21" s="166"/>
+      <c r="K21" s="164" t="s">
         <v>62</v>
       </c>
-      <c r="L21" s="146"/>
-      <c r="M21" s="146"/>
-      <c r="N21" s="146"/>
-      <c r="O21" s="156" t="s">
+      <c r="L21" s="164"/>
+      <c r="M21" s="164"/>
+      <c r="N21" s="164"/>
+      <c r="O21" s="169" t="s">
         <v>60</v>
       </c>
-      <c r="P21" s="146"/>
-      <c r="Q21" s="146"/>
-      <c r="R21" s="146"/>
-      <c r="S21" s="154" t="s">
+      <c r="P21" s="164"/>
+      <c r="Q21" s="164"/>
+      <c r="R21" s="164"/>
+      <c r="S21" s="165" t="s">
         <v>61</v>
       </c>
-      <c r="T21" s="146"/>
-      <c r="U21" s="146"/>
-      <c r="V21" s="155"/>
-      <c r="W21" s="146" t="s">
+      <c r="T21" s="164"/>
+      <c r="U21" s="164"/>
+      <c r="V21" s="166"/>
+      <c r="W21" s="164" t="s">
         <v>62</v>
       </c>
-      <c r="X21" s="146"/>
-      <c r="Y21" s="146"/>
-      <c r="Z21" s="147"/>
+      <c r="X21" s="164"/>
+      <c r="Y21" s="164"/>
+      <c r="Z21" s="170"/>
       <c r="AA21" s="108"/>
-      <c r="AD21" s="159"/>
+      <c r="AD21" s="148"/>
       <c r="AE21" s="25" t="s">
         <v>4</v>
       </c>
@@ -14793,59 +14856,59 @@
         <v>1.8422863010476525</v>
       </c>
     </row>
-    <row r="22" spans="1:35" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="108"/>
       <c r="B22" s="108"/>
-      <c r="C22" s="148" t="s">
+      <c r="C22" s="167" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="149"/>
-      <c r="E22" s="149" t="s">
+      <c r="D22" s="153"/>
+      <c r="E22" s="153" t="s">
         <v>66</v>
       </c>
-      <c r="F22" s="149"/>
-      <c r="G22" s="150" t="s">
+      <c r="F22" s="153"/>
+      <c r="G22" s="154" t="s">
         <v>65</v>
       </c>
-      <c r="H22" s="149"/>
-      <c r="I22" s="149" t="s">
+      <c r="H22" s="153"/>
+      <c r="I22" s="153" t="s">
         <v>66</v>
       </c>
-      <c r="J22" s="151"/>
-      <c r="K22" s="149" t="s">
+      <c r="J22" s="155"/>
+      <c r="K22" s="153" t="s">
         <v>65</v>
       </c>
-      <c r="L22" s="149"/>
-      <c r="M22" s="149" t="s">
+      <c r="L22" s="153"/>
+      <c r="M22" s="153" t="s">
         <v>66</v>
       </c>
-      <c r="N22" s="149"/>
+      <c r="N22" s="153"/>
       <c r="O22" s="152" t="s">
         <v>65</v>
       </c>
-      <c r="P22" s="149"/>
-      <c r="Q22" s="149" t="s">
+      <c r="P22" s="153"/>
+      <c r="Q22" s="153" t="s">
         <v>66</v>
       </c>
-      <c r="R22" s="149"/>
-      <c r="S22" s="150" t="s">
+      <c r="R22" s="153"/>
+      <c r="S22" s="154" t="s">
         <v>65</v>
       </c>
-      <c r="T22" s="149"/>
-      <c r="U22" s="149" t="s">
+      <c r="T22" s="153"/>
+      <c r="U22" s="153" t="s">
         <v>66</v>
       </c>
-      <c r="V22" s="151"/>
-      <c r="W22" s="149" t="s">
+      <c r="V22" s="155"/>
+      <c r="W22" s="153" t="s">
         <v>65</v>
       </c>
-      <c r="X22" s="149"/>
-      <c r="Y22" s="149" t="s">
+      <c r="X22" s="153"/>
+      <c r="Y22" s="153" t="s">
         <v>66</v>
       </c>
-      <c r="Z22" s="157"/>
+      <c r="Z22" s="168"/>
       <c r="AA22" s="108"/>
-      <c r="AD22" s="163"/>
+      <c r="AD22" s="151"/>
       <c r="AE22" s="57" t="s">
         <v>0</v>
       </c>
@@ -14862,7 +14925,7 @@
         <v>0.11635913277974096</v>
       </c>
     </row>
-    <row r="23" spans="1:35" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:35" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="108"/>
       <c r="B23" s="108"/>
       <c r="C23" s="28" t="s">
@@ -14939,8 +15002,8 @@
       </c>
       <c r="AA23" s="108"/>
     </row>
-    <row r="24" spans="1:35" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A24" s="161" t="s">
+    <row r="24" spans="1:35" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="138" t="s">
         <v>69</v>
       </c>
       <c r="B24" s="31" t="s">
@@ -15020,8 +15083,8 @@
       </c>
       <c r="AA24" s="108"/>
     </row>
-    <row r="25" spans="1:35" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A25" s="162"/>
+    <row r="25" spans="1:35" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="139"/>
       <c r="B25" s="124" t="s">
         <v>77</v>
       </c>
@@ -15098,17 +15161,17 @@
         <v>5285.3643541100637</v>
       </c>
       <c r="AA25" s="108"/>
-      <c r="AD25" s="137" t="s">
+      <c r="AD25" s="140" t="s">
         <v>76</v>
       </c>
-      <c r="AE25" s="138"/>
-      <c r="AF25" s="138"/>
-      <c r="AG25" s="138"/>
-      <c r="AH25" s="138"/>
-      <c r="AI25" s="139"/>
-    </row>
-    <row r="26" spans="1:35" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="162"/>
+      <c r="AE25" s="141"/>
+      <c r="AF25" s="141"/>
+      <c r="AG25" s="141"/>
+      <c r="AH25" s="141"/>
+      <c r="AI25" s="142"/>
+    </row>
+    <row r="26" spans="1:35" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="139"/>
       <c r="B26" s="41" t="s">
         <v>71</v>
       </c>
@@ -15187,17 +15250,17 @@
       <c r="AA26" s="108"/>
       <c r="AD26" s="19"/>
       <c r="AE26" s="20"/>
-      <c r="AF26" s="144" t="s">
+      <c r="AF26" s="143" t="s">
         <v>56</v>
       </c>
-      <c r="AG26" s="145"/>
+      <c r="AG26" s="144"/>
       <c r="AH26" s="21" t="s">
         <v>57</v>
       </c>
       <c r="AI26" s="22"/>
     </row>
-    <row r="27" spans="1:35" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="164" t="s">
+    <row r="27" spans="1:35" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="145" t="s">
         <v>72</v>
       </c>
       <c r="B27" s="49" t="s">
@@ -15291,8 +15354,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A28" s="162"/>
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A28" s="139"/>
       <c r="B28" s="124" t="s">
         <v>77</v>
       </c>
@@ -15369,7 +15432,7 @@
         <v>6167.6673132257747</v>
       </c>
       <c r="AA28" s="108"/>
-      <c r="AD28" s="158" t="s">
+      <c r="AD28" s="147" t="s">
         <v>2</v>
       </c>
       <c r="AE28" s="25" t="s">
@@ -15392,8 +15455,8 @@
         <v>0.38096232504700211</v>
       </c>
     </row>
-    <row r="29" spans="1:35" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="165"/>
+    <row r="29" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="146"/>
       <c r="B29" s="41" t="s">
         <v>71</v>
       </c>
@@ -15470,7 +15533,7 @@
         <v>21.650203815422461</v>
       </c>
       <c r="AA29" s="108"/>
-      <c r="AD29" s="159"/>
+      <c r="AD29" s="148"/>
       <c r="AE29" s="25" t="s">
         <v>4</v>
       </c>
@@ -15491,8 +15554,8 @@
         <v>0.3751647110073294</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A30" s="162" t="s">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A30" s="139" t="s">
         <v>73</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -15571,7 +15634,7 @@
         <v>3.5494546524051582E-2</v>
       </c>
       <c r="AA30" s="108"/>
-      <c r="AD30" s="160"/>
+      <c r="AD30" s="149"/>
       <c r="AE30" s="25" t="s">
         <v>0</v>
       </c>
@@ -15592,8 +15655,8 @@
         <v>0.38828103100666927</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A31" s="162"/>
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A31" s="139"/>
       <c r="B31" s="124" t="s">
         <v>77</v>
       </c>
@@ -15670,7 +15733,7 @@
         <v>22027.134242709195</v>
       </c>
       <c r="AA31" s="108"/>
-      <c r="AD31" s="158" t="s">
+      <c r="AD31" s="147" t="s">
         <v>1</v>
       </c>
       <c r="AE31" s="25" t="s">
@@ -15693,8 +15756,8 @@
         <v>0.34861593627624016</v>
       </c>
     </row>
-    <row r="32" spans="1:35" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A32" s="166"/>
+    <row r="32" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="150"/>
       <c r="B32" s="41" t="s">
         <v>71</v>
       </c>
@@ -15771,7 +15834,7 @@
         <v>32.948863965993311</v>
       </c>
       <c r="AA32" s="108"/>
-      <c r="AD32" s="159"/>
+      <c r="AD32" s="148"/>
       <c r="AE32" s="25" t="s">
         <v>4</v>
       </c>
@@ -15792,7 +15855,7 @@
         <v>0.35864656263191186</v>
       </c>
     </row>
-    <row r="33" spans="1:35" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:35" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="108"/>
       <c r="B33" s="108"/>
       <c r="C33" s="108"/>
@@ -15820,7 +15883,7 @@
       <c r="Y33" s="108"/>
       <c r="Z33" s="108"/>
       <c r="AA33" s="108"/>
-      <c r="AD33" s="163"/>
+      <c r="AD33" s="151"/>
       <c r="AE33" s="57" t="s">
         <v>0</v>
       </c>
@@ -15841,7 +15904,7 @@
         <v>0.3273418222518778</v>
       </c>
     </row>
-    <row r="34" spans="1:35" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:35" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C34" s="116"/>
       <c r="D34" s="116"/>
       <c r="E34" s="116"/>
@@ -15850,7 +15913,7 @@
       <c r="H34" s="116"/>
       <c r="I34" s="116"/>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C35" s="116"/>
       <c r="D35" s="116"/>
       <c r="E35" s="116"/>
@@ -15859,7 +15922,7 @@
       <c r="H35" s="116"/>
       <c r="I35" s="116"/>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C36" s="116"/>
       <c r="D36" s="116"/>
       <c r="E36" s="116"/>
@@ -15868,7 +15931,7 @@
       <c r="H36" s="116"/>
       <c r="I36" s="116"/>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C37" s="119"/>
       <c r="D37" s="116"/>
       <c r="E37" s="116"/>
@@ -15877,7 +15940,7 @@
       <c r="H37" s="116"/>
       <c r="I37" s="116"/>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C38" s="116"/>
       <c r="D38" s="116"/>
       <c r="E38" s="116"/>
@@ -15886,7 +15949,7 @@
       <c r="H38" s="116"/>
       <c r="I38" s="116"/>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C39" s="118"/>
       <c r="D39" s="118"/>
       <c r="E39" s="118"/>
@@ -15912,7 +15975,7 @@
       <c r="Y39" s="109"/>
       <c r="Z39" s="109"/>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C40" s="118"/>
       <c r="D40" s="118"/>
       <c r="E40" s="118"/>
@@ -15938,7 +16001,7 @@
       <c r="Y40" s="109"/>
       <c r="Z40" s="109"/>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C41" s="118"/>
       <c r="D41" s="118"/>
       <c r="E41" s="118"/>
@@ -15964,7 +16027,7 @@
       <c r="Y41" s="109"/>
       <c r="Z41" s="109"/>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C42" s="118"/>
       <c r="D42" s="118"/>
       <c r="E42" s="118"/>
@@ -15990,7 +16053,7 @@
       <c r="Y42" s="109"/>
       <c r="Z42" s="109"/>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C43" s="108"/>
       <c r="D43" s="108"/>
       <c r="E43" s="108"/>
@@ -16016,28 +16079,38 @@
       <c r="Y43" s="108"/>
       <c r="Z43" s="108"/>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" s="119"/>
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="AD25:AI25"/>
-    <mergeCell ref="AF26:AG26"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="AD28:AD30"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="AD31:AD33"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="W22:X22"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="AD14:AI14"/>
-    <mergeCell ref="AF15:AG15"/>
-    <mergeCell ref="AD17:AD19"/>
-    <mergeCell ref="C19:Z19"/>
+    <mergeCell ref="C3:Z3"/>
+    <mergeCell ref="AD3:AI3"/>
+    <mergeCell ref="C4:N4"/>
+    <mergeCell ref="O4:Z4"/>
+    <mergeCell ref="AF4:AG4"/>
+    <mergeCell ref="W5:Z5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="O5:R5"/>
+    <mergeCell ref="S5:V5"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="AD6:AD8"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="AD9:AD11"/>
+    <mergeCell ref="A11:A13"/>
     <mergeCell ref="C20:N20"/>
     <mergeCell ref="O20:Z20"/>
     <mergeCell ref="AD20:AD22"/>
@@ -16054,33 +16127,23 @@
     <mergeCell ref="S21:V21"/>
     <mergeCell ref="W21:Z21"/>
     <mergeCell ref="M22:N22"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="AD6:AD8"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="AD9:AD11"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="W5:Z5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="O5:R5"/>
-    <mergeCell ref="S5:V5"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="C3:Z3"/>
-    <mergeCell ref="AD3:AI3"/>
-    <mergeCell ref="C4:N4"/>
-    <mergeCell ref="O4:Z4"/>
-    <mergeCell ref="AF4:AG4"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="AD14:AI14"/>
+    <mergeCell ref="AF15:AG15"/>
+    <mergeCell ref="AD17:AD19"/>
+    <mergeCell ref="C19:Z19"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="W22:X22"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="AD25:AI25"/>
+    <mergeCell ref="AF26:AG26"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="AD28:AD30"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="AD31:AD33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>